<commit_message>
Fase 3 final relatorio
</commit_message>
<xml_diff>
--- a/Fase3/IC_Project_Fase3_Grid_Excel.xlsx
+++ b/Fase3/IC_Project_Fase3_Grid_Excel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luist\OneDrive\Ambiente de Trabalho\ISEC\ano3_EngInformatica\IC\IC_PraticalWork\Fase3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A3672F-1F8D-4C02-9ABD-230BF9E488B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formas dos Conjuntos" sheetId="1" r:id="rId1"/>
@@ -13,12 +19,12 @@
     <sheet name="Relatório de Classificação" sheetId="4" r:id="rId4"/>
     <sheet name="AUC por Classe" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Conjunto</t>
   </si>
@@ -159,13 +165,16 @@
   </si>
   <si>
     <t>AUC</t>
+  </si>
+  <si>
+    <t>Numero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,24 +226,1132 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Perda Grid Search</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Resultados Otimizacao'!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Resultados Otimizacao'!$C$2:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.534330000480016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29918789863586431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13362864653269449</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22111479441324869</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20524179935455319</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5756736695766449</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24381691217422491</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2122554580370585</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2511997024218241</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33831671873728431</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65300848086675001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.30786267916361493</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.10262087980906159</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.21299372116724649</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.37006274859110511</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.60520487030347181</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.32225912809371948</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.212809165318807</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.23606497049331671</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2209302385648092</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.72388335069020582</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.29844961563746131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.6378733317057255E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.12587672472000119</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.17349576950073239</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6E70-478F-830D-2FE7EF1EC7B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="315"/>
+        <c:overlap val="-40"/>
+        <c:axId val="2140046671"/>
+        <c:axId val="2021183583"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2140046671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2021183583"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2021183583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2140046671"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ACABAB3-C574-5C31-9020-5703F23CFD95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5E8185E-6AB7-43D7-92F7-A18D1ABFBCEA}" name="Tabela1" displayName="Tabela1" ref="A1:C26" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C26" xr:uid="{C5E8185E-6AB7-43D7-92F7-A18D1ABFBCEA}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{AA7A1FBD-6AE0-489A-8093-603AA25D6FC5}" name="Numero"/>
+    <tableColumn id="2" xr3:uid="{4FCE39A7-A8E2-4943-BA16-B67E448BE384}" name="Hiperparâmetros"/>
+    <tableColumn id="3" xr3:uid="{073981AE-3B0C-4CA5-96FF-BD9514DC7DA4}" name="Perda"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -272,7 +1389,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -306,6 +1423,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -340,9 +1458,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -515,14 +1634,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -538,7 +1657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -546,7 +1665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -560,235 +1679,324 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.534330000480016</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>0.2991878986358643</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="C3">
+        <v>0.29918789863586431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>0.1336286465326945</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="C4">
+        <v>0.13362864653269449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
-        <v>0.2211147944132487</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="C5">
+        <v>0.22111479441324869</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
-        <v>0.2052417993545532</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="C6">
+        <v>0.20524179935455319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.5756736695766449</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
-        <v>0.2438169121742249</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="C8">
+        <v>0.24381691217422491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.2122554580370585</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.2511997024218241</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="B11">
-        <v>0.3383167187372843</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="C11">
+        <v>0.33831671873728431</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="B12">
-        <v>0.65300848086675</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="C12">
+        <v>0.65300848086675001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="B13">
-        <v>0.3078626791636149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="C13">
+        <v>0.30786267916361493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="B14">
-        <v>0.1026208798090616</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="C14">
+        <v>0.10262087980906159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="B15">
-        <v>0.2129937211672465</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="C15">
+        <v>0.21299372116724649</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="B16">
-        <v>0.3700627485911051</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="C16">
+        <v>0.37006274859110511</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
-        <v>0.6052048703034718</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="C17">
+        <v>0.60520487030347181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
-        <v>0.3222591280937195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="C18">
+        <v>0.32225912809371948</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>0.212809165318807</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="B20">
-        <v>0.2360649704933167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="C20">
+        <v>0.23606497049331671</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>0.2209302385648092</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="B22">
-        <v>0.7238833506902058</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="C22">
+        <v>0.72388335069020582</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="B23">
-        <v>0.2984496156374613</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="C23">
+        <v>0.29844961563746131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="B24">
-        <v>0.08637873331705725</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="C24">
+        <v>8.6378733317057255E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>33</v>
       </c>
-      <c r="B25">
-        <v>0.1258767247200012</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="C25">
+        <v>0.12587672472000119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="B26">
-        <v>0.1734957695007324</v>
+      <c r="C26">
+        <v>0.17349576950073239</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
@@ -799,7 +2007,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -813,7 +2021,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -827,7 +2035,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -847,14 +2055,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
@@ -868,103 +2076,103 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B2">
-        <v>0.8914473684210527</v>
+        <v>0.89144736842105265</v>
       </c>
       <c r="C2">
-        <v>0.7424657534246575</v>
+        <v>0.74246575342465748</v>
       </c>
       <c r="D2">
-        <v>0.8101644245142002</v>
+        <v>0.81016442451420023</v>
       </c>
       <c r="E2">
         <v>365</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B3">
-        <v>0.8653846153846154</v>
+        <v>0.86538461538461542</v>
       </c>
       <c r="C3">
         <v>0.7917888563049853</v>
       </c>
       <c r="D3">
-        <v>0.8269525267993875</v>
+        <v>0.82695252679938747</v>
       </c>
       <c r="E3">
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B4">
-        <v>0.7935483870967742</v>
+        <v>0.79354838709677422</v>
       </c>
       <c r="C4">
-        <v>0.984</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="D4">
-        <v>0.8785714285714286</v>
+        <v>0.87857142857142856</v>
       </c>
       <c r="E4">
         <v>375</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B5">
-        <v>0.8418131359851989</v>
+        <v>0.84181313598519891</v>
       </c>
       <c r="C5">
-        <v>0.8418131359851989</v>
+        <v>0.84181313598519891</v>
       </c>
       <c r="D5">
-        <v>0.8418131359851989</v>
+        <v>0.84181313598519891</v>
       </c>
       <c r="E5">
-        <v>0.8418131359851989</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0.84181313598519891</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B6">
-        <v>0.8501267903008141</v>
+        <v>0.85012679030081406</v>
       </c>
       <c r="C6">
-        <v>0.8394182032432141</v>
+        <v>0.83941820324321414</v>
       </c>
       <c r="D6">
-        <v>0.8385627932950054</v>
+        <v>0.83856279329500538</v>
       </c>
       <c r="E6">
         <v>1081</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B7">
-        <v>0.8492646516939208</v>
+        <v>0.84926465169392085</v>
       </c>
       <c r="C7">
-        <v>0.8418131359851989</v>
+        <v>0.84181313598519891</v>
       </c>
       <c r="D7">
-        <v>0.8391906681781313</v>
+        <v>0.83919066817813126</v>
       </c>
       <c r="E7">
         <v>1081</v>
@@ -976,14 +2184,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -991,28 +2199,28 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2">
-        <v>0.9535145787097267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>0.95351457870972667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
       <c r="B3">
-        <v>0.9588709677419355</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>0.95887096774193548</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4">
-        <v>0.9893408876298395</v>
+        <v>0.98934088762983952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>